<commit_message>
chore(data): update classifica workbook
</commit_message>
<xml_diff>
--- a/Classifica_FantaPortoscuso-25.xlsx
+++ b/Classifica_FantaPortoscuso-25.xlsx
@@ -50,235 +50,235 @@
     <t>F.C Pennic Hellas</t>
   </si>
   <si>
+    <t>Scarzooka</t>
+  </si>
+  <si>
     <t>MARCIO TEAM</t>
   </si>
   <si>
-    <t>Scarzooka</t>
-  </si>
-  <si>
     <t>Collocolo Team</t>
   </si>
   <si>
+    <t>TomMat-iga</t>
+  </si>
+  <si>
+    <t>FC Plasmon</t>
+  </si>
+  <si>
+    <t>Antibro</t>
+  </si>
+  <si>
+    <t>FC Galli</t>
+  </si>
+  <si>
+    <t>FC Spiaze</t>
+  </si>
+  <si>
     <t>Plu-Team</t>
   </si>
   <si>
-    <t>Antibro</t>
-  </si>
-  <si>
-    <t>TomMat-iga</t>
-  </si>
-  <si>
-    <t>FC Spiaze</t>
+    <t>Non troppo cattivi</t>
+  </si>
+  <si>
+    <t>I COMPARI</t>
+  </si>
+  <si>
+    <t>Pro secco</t>
+  </si>
+  <si>
+    <t>Ipa Bali</t>
+  </si>
+  <si>
+    <t>Lunarossa</t>
+  </si>
+  <si>
+    <t>DonBosko46</t>
+  </si>
+  <si>
+    <t>LE 4 M</t>
+  </si>
+  <si>
+    <t>SPERA EBBASTA</t>
   </si>
   <si>
     <t>BOBONE32</t>
   </si>
   <si>
+    <t>Imperatori del culo</t>
+  </si>
+  <si>
+    <t>ISGOPPAISI2</t>
+  </si>
+  <si>
     <t>Leonte FC</t>
   </si>
   <si>
-    <t>FC Plasmon</t>
-  </si>
-  <si>
-    <t>FC Galli</t>
-  </si>
-  <si>
-    <t>Pro secco</t>
+    <t>XLiverpuh</t>
   </si>
   <si>
     <t>OnlyFans</t>
   </si>
   <si>
-    <t>ISGOPPAISI2</t>
-  </si>
-  <si>
-    <t>I COMPARI</t>
-  </si>
-  <si>
-    <t>XLiverpuh</t>
-  </si>
-  <si>
-    <t>Ipa Bali</t>
-  </si>
-  <si>
-    <t>Non troppo cattivi</t>
-  </si>
-  <si>
-    <t>Lunarossa</t>
-  </si>
-  <si>
-    <t>SPERA EBBASTA</t>
-  </si>
-  <si>
-    <t>LE 4 M</t>
-  </si>
-  <si>
-    <t>DonBosko46</t>
-  </si>
-  <si>
-    <t>Imperatori del culo</t>
+    <t>Temptation Haaland</t>
   </si>
   <si>
     <t>Pi-Ciaccio</t>
   </si>
   <si>
+    <t>AC DENTI</t>
+  </si>
+  <si>
     <t>BARAKALLAHOUFIK</t>
   </si>
   <si>
+    <t>Due Amici al Var</t>
+  </si>
+  <si>
     <t>Concali Craboni FC</t>
   </si>
   <si>
+    <t>Boiali</t>
+  </si>
+  <si>
+    <t>A.C.TUA CUCS</t>
+  </si>
+  <si>
+    <t>coach 71</t>
+  </si>
+  <si>
+    <t>Hellas merdona</t>
+  </si>
+  <si>
+    <t>PEAKY BLINDERS</t>
+  </si>
+  <si>
+    <t>i bro</t>
+  </si>
+  <si>
+    <t>scarsenal</t>
+  </si>
+  <si>
+    <t>Peaky Tunas</t>
+  </si>
+  <si>
     <t>SILVEDO</t>
   </si>
   <si>
-    <t>A.C.TUA CUCS</t>
-  </si>
-  <si>
-    <t>Peaky Tunas</t>
-  </si>
-  <si>
-    <t>Due Amici al Var</t>
-  </si>
-  <si>
-    <t>Temptation Haaland</t>
-  </si>
-  <si>
-    <t>AC DENTI</t>
-  </si>
-  <si>
-    <t>PEAKY BLINDERS</t>
-  </si>
-  <si>
-    <t>Boiali</t>
+    <t>SPOSTATI</t>
+  </si>
+  <si>
+    <t>Giubbentus</t>
+  </si>
+  <si>
+    <t>Malmö FF</t>
+  </si>
+  <si>
+    <t>Sarzanello Team</t>
+  </si>
+  <si>
+    <t>BinuSpuntu</t>
   </si>
   <si>
     <t>BANDITI</t>
   </si>
   <si>
-    <t>Malmö FF</t>
-  </si>
-  <si>
-    <t>Giubbentus</t>
-  </si>
-  <si>
-    <t>Hellas merdona</t>
-  </si>
-  <si>
-    <t>Sarzanello Team</t>
-  </si>
-  <si>
-    <t>SPOSTATI</t>
-  </si>
-  <si>
-    <t>scarsenal</t>
-  </si>
-  <si>
-    <t>coach 71</t>
-  </si>
-  <si>
-    <t>i bro</t>
-  </si>
-  <si>
     <t>Real Mellandro</t>
   </si>
   <si>
+    <t>Nastro Azzurro</t>
+  </si>
+  <si>
+    <t>LosPollosHermanos</t>
+  </si>
+  <si>
     <t>puerto rosso blu</t>
   </si>
   <si>
+    <t>Longobarda</t>
+  </si>
+  <si>
+    <t>SAGATU</t>
+  </si>
+  <si>
+    <t>KARABE 1975</t>
+  </si>
+  <si>
+    <t>Sciabolata Classica</t>
+  </si>
+  <si>
+    <t>SerSi-FC</t>
+  </si>
+  <si>
+    <t>Piovra73</t>
+  </si>
+  <si>
     <t>Riccardigno</t>
   </si>
   <si>
-    <t>BinuSpuntu</t>
-  </si>
-  <si>
-    <t>Longobarda</t>
-  </si>
-  <si>
-    <t>SAGATU</t>
+    <t>Sisal Palace</t>
+  </si>
+  <si>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>buttiglia25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuginiDiCampagna </t>
+  </si>
+  <si>
+    <t>FC Buttarighe</t>
+  </si>
+  <si>
+    <t>pacho team</t>
   </si>
   <si>
     <t>LEONE</t>
   </si>
   <si>
-    <t>Nastro Azzurro</t>
-  </si>
-  <si>
-    <t>Piovra73</t>
-  </si>
-  <si>
-    <t>LosPollosHermanos</t>
-  </si>
-  <si>
-    <t>Lions</t>
-  </si>
-  <si>
-    <t>KARABE 1975</t>
-  </si>
-  <si>
-    <t>pacho team</t>
-  </si>
-  <si>
-    <t>Sciabolata Classica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CuginiDiCampagna </t>
-  </si>
-  <si>
-    <t>SerSi-FC</t>
-  </si>
-  <si>
-    <t>buttiglia25</t>
-  </si>
-  <si>
     <t>ROCKY 3</t>
   </si>
   <si>
+    <t>SMOG</t>
+  </si>
+  <si>
+    <t>lagg</t>
+  </si>
+  <si>
+    <t>i fratelli merda</t>
+  </si>
+  <si>
+    <t>Fc nipiri</t>
+  </si>
+  <si>
+    <t>Mapoitta</t>
+  </si>
+  <si>
+    <t>kalashnikov</t>
+  </si>
+  <si>
     <t>CISCO TEAM</t>
   </si>
   <si>
-    <t>Fc nipiri</t>
-  </si>
-  <si>
-    <t>SMOG</t>
-  </si>
-  <si>
-    <t>Sisal Palace</t>
-  </si>
-  <si>
-    <t>i fratelli merda</t>
-  </si>
-  <si>
-    <t>FC Buttarighe</t>
-  </si>
-  <si>
-    <t>lagg</t>
+    <t>I Cigni</t>
+  </si>
+  <si>
+    <t>CLAN</t>
+  </si>
+  <si>
+    <t>Kung-Fu Pandev</t>
   </si>
   <si>
     <t>DEEDPULLY</t>
   </si>
   <si>
-    <t>kalashnikov</t>
-  </si>
-  <si>
     <t>real donk</t>
   </si>
   <si>
-    <t>Mapoitta</t>
-  </si>
-  <si>
-    <t>I Cigni</t>
-  </si>
-  <si>
-    <t>Kung-Fu Pandev</t>
+    <t>ProPro Proibito</t>
   </si>
   <si>
     <t>mezzebirre</t>
-  </si>
-  <si>
-    <t>CLAN</t>
-  </si>
-  <si>
-    <t>ProPro Proibito</t>
   </si>
   <si>
     <t>HeineKean</t>
@@ -432,10 +432,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7">
-        <v>1769.5</v>
+        <v>1852.5</v>
       </c>
     </row>
     <row r="6">
@@ -449,10 +449,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="7">
-        <v>1751</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="7">
@@ -466,10 +466,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="7">
-        <v>1751</v>
+        <v>1837.5</v>
       </c>
     </row>
     <row r="8">
@@ -483,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="7">
-        <v>1736</v>
+        <v>1821.5</v>
       </c>
     </row>
     <row r="9">
@@ -500,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="7">
-        <v>1730.5</v>
+        <v>1816.5</v>
       </c>
     </row>
     <row r="10">
@@ -517,10 +517,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="7">
-        <v>1727.5</v>
+        <v>1812.5</v>
       </c>
     </row>
     <row r="11">
@@ -534,10 +534,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="7">
-        <v>1725.5</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="12">
@@ -551,10 +551,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="7">
-        <v>1723</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="13">
@@ -568,10 +568,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="7">
-        <v>1714.5</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="14">
@@ -585,10 +585,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="7">
-        <v>1710.5</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="15">
@@ -602,10 +602,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7">
-        <v>1708.5</v>
+        <v>1793.5</v>
       </c>
     </row>
     <row r="16">
@@ -619,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7">
-        <v>1703</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="17">
@@ -636,10 +636,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="7">
-        <v>1702.5</v>
+        <v>1788.5</v>
       </c>
     </row>
     <row r="18">
@@ -653,10 +653,10 @@
         <v>4</v>
       </c>
       <c r="D18" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="7">
-        <v>1702</v>
+        <v>1784.5</v>
       </c>
     </row>
     <row r="19">
@@ -670,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="7">
-        <v>1700.5</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="20">
@@ -687,10 +687,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E20" s="7">
-        <v>1697</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="21">
@@ -704,10 +704,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E21" s="7">
-        <v>1697</v>
+        <v>1781.5</v>
       </c>
     </row>
     <row r="22">
@@ -721,10 +721,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="7">
-        <v>1697</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="23">
@@ -738,10 +738,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="7">
-        <v>1697</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="24">
@@ -755,10 +755,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="7">
-        <v>1696.5</v>
+        <v>1779.5</v>
       </c>
     </row>
     <row r="25">
@@ -772,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="7">
-        <v>1696.5</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="26">
@@ -789,10 +789,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="7">
-        <v>1695</v>
+        <v>1778.5</v>
       </c>
     </row>
     <row r="27">
@@ -806,10 +806,10 @@
         <v>4</v>
       </c>
       <c r="D27" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E27" s="7">
-        <v>1694</v>
+        <v>1778.5</v>
       </c>
     </row>
     <row r="28">
@@ -823,10 +823,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="7">
-        <v>1694</v>
+        <v>1777.5</v>
       </c>
     </row>
     <row r="29">
@@ -840,10 +840,10 @@
         <v>4</v>
       </c>
       <c r="D29" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E29" s="7">
-        <v>1692</v>
+        <v>1777.5</v>
       </c>
     </row>
     <row r="30">
@@ -857,10 +857,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" s="7">
-        <v>1691.5</v>
+        <v>1775.5</v>
       </c>
     </row>
     <row r="31">
@@ -874,10 +874,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31" s="7">
-        <v>1691</v>
+        <v>1775.5</v>
       </c>
     </row>
     <row r="32">
@@ -891,10 +891,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="7">
-        <v>1690.5</v>
+        <v>1767.5</v>
       </c>
     </row>
     <row r="33">
@@ -908,10 +908,10 @@
         <v>4</v>
       </c>
       <c r="D33" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E33" s="7">
-        <v>1686.5</v>
+        <v>1767.5</v>
       </c>
     </row>
     <row r="34">
@@ -925,10 +925,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E34" s="7">
-        <v>1682.5</v>
+        <v>1766.5</v>
       </c>
     </row>
     <row r="35">
@@ -942,10 +942,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E35" s="7">
-        <v>1682</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="36">
@@ -959,10 +959,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E36" s="7">
-        <v>1680</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="37">
@@ -976,10 +976,10 @@
         <v>4</v>
       </c>
       <c r="D37" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E37" s="7">
-        <v>1680</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="38">
@@ -993,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="D38" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E38" s="7">
-        <v>1678</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="39">
@@ -1010,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="D39" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="7">
-        <v>1676.5</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="40">
@@ -1027,10 +1027,10 @@
         <v>4</v>
       </c>
       <c r="D40" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" s="7">
-        <v>1676</v>
+        <v>1754.5</v>
       </c>
     </row>
     <row r="41">
@@ -1044,10 +1044,10 @@
         <v>4</v>
       </c>
       <c r="D41" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E41" s="7">
-        <v>1676</v>
+        <v>1751.5</v>
       </c>
     </row>
     <row r="42">
@@ -1061,10 +1061,10 @@
         <v>4</v>
       </c>
       <c r="D42" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E42" s="7">
-        <v>1675.5</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="43">
@@ -1078,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="D43" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E43" s="7">
-        <v>1671</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="44">
@@ -1095,10 +1095,10 @@
         <v>4</v>
       </c>
       <c r="D44" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E44" s="7">
-        <v>1671</v>
+        <v>1746.5</v>
       </c>
     </row>
     <row r="45">
@@ -1112,10 +1112,10 @@
         <v>4</v>
       </c>
       <c r="D45" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E45" s="7">
-        <v>1671</v>
+        <v>1746.5</v>
       </c>
     </row>
     <row r="46">
@@ -1129,10 +1129,10 @@
         <v>4</v>
       </c>
       <c r="D46" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E46" s="7">
-        <v>1669.5</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="47">
@@ -1146,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="D47" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E47" s="7">
-        <v>1668</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="48">
@@ -1163,10 +1163,10 @@
         <v>4</v>
       </c>
       <c r="D48" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E48" s="7">
-        <v>1668</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="49">
@@ -1180,10 +1180,10 @@
         <v>4</v>
       </c>
       <c r="D49" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E49" s="7">
-        <v>1662.5</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="50">
@@ -1197,10 +1197,10 @@
         <v>4</v>
       </c>
       <c r="D50" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E50" s="7">
-        <v>1660.5</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="51">
@@ -1214,10 +1214,10 @@
         <v>4</v>
       </c>
       <c r="D51" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E51" s="7">
-        <v>1659</v>
+        <v>1741.5</v>
       </c>
     </row>
     <row r="52">
@@ -1231,10 +1231,10 @@
         <v>4</v>
       </c>
       <c r="D52" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E52" s="7">
-        <v>1659</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="53">
@@ -1248,10 +1248,10 @@
         <v>4</v>
       </c>
       <c r="D53" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E53" s="7">
-        <v>1657</v>
+        <v>1738.5</v>
       </c>
     </row>
     <row r="54">
@@ -1265,10 +1265,10 @@
         <v>4</v>
       </c>
       <c r="D54" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E54" s="7">
-        <v>1655</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="55">
@@ -1282,10 +1282,10 @@
         <v>4</v>
       </c>
       <c r="D55" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E55" s="7">
-        <v>1654</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="56">
@@ -1299,10 +1299,10 @@
         <v>4</v>
       </c>
       <c r="D56" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E56" s="7">
-        <v>1653</v>
+        <v>1732.5</v>
       </c>
     </row>
     <row r="57">
@@ -1316,10 +1316,10 @@
         <v>4</v>
       </c>
       <c r="D57" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E57" s="7">
-        <v>1652.5</v>
+        <v>1731.5</v>
       </c>
     </row>
     <row r="58">
@@ -1333,10 +1333,10 @@
         <v>4</v>
       </c>
       <c r="D58" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E58" s="7">
-        <v>1652</v>
+        <v>1728.5</v>
       </c>
     </row>
     <row r="59">
@@ -1350,10 +1350,10 @@
         <v>4</v>
       </c>
       <c r="D59" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E59" s="7">
-        <v>1650.5</v>
+        <v>1728.5</v>
       </c>
     </row>
     <row r="60">
@@ -1367,10 +1367,10 @@
         <v>4</v>
       </c>
       <c r="D60" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E60" s="7">
-        <v>1648</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="61">
@@ -1384,10 +1384,10 @@
         <v>4</v>
       </c>
       <c r="D61" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E61" s="7">
-        <v>1643.5</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="62">
@@ -1401,10 +1401,10 @@
         <v>4</v>
       </c>
       <c r="D62" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E62" s="7">
-        <v>1642</v>
+        <v>1723.5</v>
       </c>
     </row>
     <row r="63">
@@ -1418,10 +1418,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E63" s="7">
-        <v>1641.5</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="64">
@@ -1435,10 +1435,10 @@
         <v>4</v>
       </c>
       <c r="D64" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E64" s="7">
-        <v>1641</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="65">
@@ -1452,10 +1452,10 @@
         <v>4</v>
       </c>
       <c r="D65" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E65" s="7">
-        <v>1640</v>
+        <v>1718.5</v>
       </c>
     </row>
     <row r="66">
@@ -1469,10 +1469,10 @@
         <v>4</v>
       </c>
       <c r="D66" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E66" s="7">
-        <v>1640</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="67">
@@ -1486,10 +1486,10 @@
         <v>4</v>
       </c>
       <c r="D67" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E67" s="7">
-        <v>1639.5</v>
+        <v>1717.5</v>
       </c>
     </row>
     <row r="68">
@@ -1503,10 +1503,10 @@
         <v>4</v>
       </c>
       <c r="D68" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E68" s="7">
-        <v>1639.5</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="69">
@@ -1520,10 +1520,10 @@
         <v>4</v>
       </c>
       <c r="D69" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E69" s="7">
-        <v>1636.5</v>
+        <v>1712.5</v>
       </c>
     </row>
     <row r="70">
@@ -1537,10 +1537,10 @@
         <v>4</v>
       </c>
       <c r="D70" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E70" s="7">
-        <v>1636</v>
+        <v>1711.5</v>
       </c>
     </row>
     <row r="71">
@@ -1554,10 +1554,10 @@
         <v>4</v>
       </c>
       <c r="D71" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E71" s="7">
-        <v>1631</v>
+        <v>1711.5</v>
       </c>
     </row>
     <row r="72">
@@ -1571,10 +1571,10 @@
         <v>4</v>
       </c>
       <c r="D72" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E72" s="7">
-        <v>1629.5</v>
+        <v>1708.5</v>
       </c>
     </row>
     <row r="73">
@@ -1588,10 +1588,10 @@
         <v>4</v>
       </c>
       <c r="D73" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E73" s="7">
-        <v>1629</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="74">
@@ -1605,10 +1605,10 @@
         <v>4</v>
       </c>
       <c r="D74" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E74" s="7">
-        <v>1628.5</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="75">
@@ -1622,10 +1622,10 @@
         <v>4</v>
       </c>
       <c r="D75" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E75" s="7">
-        <v>1628</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="76">
@@ -1639,10 +1639,10 @@
         <v>4</v>
       </c>
       <c r="D76" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E76" s="7">
-        <v>1626</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="77">
@@ -1656,10 +1656,10 @@
         <v>4</v>
       </c>
       <c r="D77" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E77" s="7">
-        <v>1624.5</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="78">
@@ -1673,10 +1673,10 @@
         <v>4</v>
       </c>
       <c r="D78" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E78" s="7">
-        <v>1622.5</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="79">
@@ -1690,10 +1690,10 @@
         <v>4</v>
       </c>
       <c r="D79" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E79" s="7">
-        <v>1622.5</v>
+        <v>1699.5</v>
       </c>
     </row>
     <row r="80">
@@ -1707,10 +1707,10 @@
         <v>4</v>
       </c>
       <c r="D80" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E80" s="7">
-        <v>1620.5</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="81">
@@ -1724,10 +1724,10 @@
         <v>4</v>
       </c>
       <c r="D81" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E81" s="7">
-        <v>1615</v>
+        <v>1697.5</v>
       </c>
     </row>
     <row r="82">
@@ -1741,10 +1741,10 @@
         <v>4</v>
       </c>
       <c r="D82" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E82" s="7">
-        <v>1614.5</v>
+        <v>1697.5</v>
       </c>
     </row>
     <row r="83">
@@ -1758,10 +1758,10 @@
         <v>4</v>
       </c>
       <c r="D83" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E83" s="7">
-        <v>1612.5</v>
+        <v>1696.5</v>
       </c>
     </row>
     <row r="84">
@@ -1775,10 +1775,10 @@
         <v>4</v>
       </c>
       <c r="D84" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E84" s="7">
-        <v>1608.5</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="85">
@@ -1792,10 +1792,10 @@
         <v>4</v>
       </c>
       <c r="D85" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E85" s="7">
-        <v>1602.5</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="86">
@@ -1809,10 +1809,10 @@
         <v>4</v>
       </c>
       <c r="D86" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E86" s="7">
-        <v>1596.5</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="87">
@@ -1826,10 +1826,10 @@
         <v>4</v>
       </c>
       <c r="D87" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E87" s="7">
-        <v>1580</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="88">
@@ -1843,10 +1843,10 @@
         <v>4</v>
       </c>
       <c r="D88" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E88" s="7">
-        <v>1573</v>
+        <v>1641.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>